<commit_message>
add note to subnetting chart
</commit_message>
<xml_diff>
--- a/SubnettingChartRedux.xlsx
+++ b/SubnettingChartRedux.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="330">
   <si>
     <t>.8</t>
   </si>
@@ -1037,6 +1037,9 @@
   </si>
   <si>
     <t># Hosts per Network</t>
+  </si>
+  <si>
+    <t>Note: GW value assumes first usable address in range.</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1518,6 +1521,7 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1759,8 +1763,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A72:G77" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="A72:G77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A76:G81" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="A76:G81">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2045,10 +2049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H77"/>
+  <dimension ref="A2:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,142 +3467,145 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="16"/>
-    </row>
-    <row r="72" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="52" t="s">
+      <c r="B71" s="54" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="52" t="s">
         <v>301</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B76" s="53" t="s">
         <v>313</v>
       </c>
-      <c r="C72" s="53" t="s">
+      <c r="C76" s="53" t="s">
         <v>312</v>
       </c>
-      <c r="D72" s="53" t="s">
+      <c r="D76" s="53" t="s">
         <v>319</v>
       </c>
-      <c r="E72" s="53" t="s">
+      <c r="E76" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="F72" s="53" t="s">
+      <c r="F76" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="G72" s="53" t="s">
+      <c r="G76" s="53" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="36" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="36" t="s">
         <v>302</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B77" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="C73" s="38" t="s">
+      <c r="C77" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="D73" s="39" t="s">
+      <c r="D77" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E77" s="40" t="s">
         <v>324</v>
       </c>
-      <c r="F73" s="41">
+      <c r="F77" s="41">
         <v>127</v>
       </c>
-      <c r="G73" s="42">
+      <c r="G77" s="42">
         <v>16777214</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="43" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="43" t="s">
         <v>303</v>
       </c>
-      <c r="B74" s="44" t="s">
+      <c r="B78" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C78" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="D74" s="46" t="s">
+      <c r="D78" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="E74" s="47" t="s">
+      <c r="E78" s="47" t="s">
         <v>325</v>
       </c>
-      <c r="F74" s="48">
+      <c r="F78" s="48">
         <v>16384</v>
       </c>
-      <c r="G74" s="49">
+      <c r="G78" s="49">
         <v>65534</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="43" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B75" s="44" t="s">
+      <c r="B79" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="C79" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="D75" s="46" t="s">
+      <c r="D79" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="E75" s="47" t="s">
+      <c r="E79" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="F75" s="48">
+      <c r="F79" s="48">
         <v>2097152</v>
       </c>
-      <c r="G75" s="49">
+      <c r="G79" s="49">
         <v>254</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="43" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B76" s="44" t="s">
+      <c r="B80" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C80" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="D76" s="46" t="s">
+      <c r="D80" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="E76" s="46" t="s">
+      <c r="E80" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="F76" s="46" t="s">
+      <c r="F80" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="G76" s="50" t="s">
+      <c r="G80" s="50" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="51" t="s">
+    <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="B77" s="44" t="s">
+      <c r="B81" s="44" t="s">
         <v>311</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C81" s="45" t="s">
         <v>318</v>
       </c>
-      <c r="D77" s="46" t="s">
+      <c r="D81" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="E77" s="46" t="s">
+      <c r="E81" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="F77" s="46" t="s">
+      <c r="F81" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="G77" s="50" t="s">
+      <c r="G81" s="50" t="s">
         <v>323</v>
       </c>
     </row>

</xml_diff>